<commit_message>
mechanics filtered by grouping
</commit_message>
<xml_diff>
--- a/BGGData/MechanicsGrouping.xlsx
+++ b/BGGData/MechanicsGrouping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\GitSources\BGGMechsAndRatings\BGGData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A08805-8DBC-4BD6-B4F4-9E10FEAAC7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4927CECF-0D33-448F-BD9D-4293A46C1BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4188" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,7 @@
   <dimension ref="A1:B192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1183,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -2046,5 +2046,6 @@
     <sortCondition ref="A2:A192"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>